<commit_message>
Se back actualizado con el .env
</commit_message>
<xml_diff>
--- a/marcaciones.xlsx
+++ b/marcaciones.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -902,9 +902,89 @@
         <v>Gracias</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>jamilton</v>
+      </c>
+      <c r="B26" t="str">
+        <v>7878</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Alameda</v>
+      </c>
+      <c r="D26" t="str">
+        <v>22/05/2025, 14:57:09</v>
+      </c>
+      <c r="E26" t="str">
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <v>hou</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>David</v>
+      </c>
+      <c r="B27" t="str">
+        <v>1265</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Neiva</v>
+      </c>
+      <c r="D27" t="str">
+        <v>29/05/2025, 09:50:42</v>
+      </c>
+      <c r="E27" t="str">
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <v>aaa</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Goliat</v>
+      </c>
+      <c r="B28" t="str">
+        <v>14569</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Cafetero</v>
+      </c>
+      <c r="D28" t="str">
+        <v>29/05/2025, 10:06:14</v>
+      </c>
+      <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <v>Llegue tarde</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B29" t="str">
+        <v>1006036679</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Delicias</v>
+      </c>
+      <c r="D29" t="str">
+        <v>28/05/2025, 10:07:46</v>
+      </c>
+      <c r="E29" t="str">
+        <v>28/05/2025, 10:07:46</v>
+      </c>
+      <c r="F29" t="str">
+        <v>HGola</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>